<commit_message>
Modified Controller functions to generate role based xlsx and csv reports
</commit_message>
<xml_diff>
--- a/docs/characters.xlsx
+++ b/docs/characters.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -427,7 +427,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>64d26c9307ffbcb398e2516c</v>
+        <v>64d679773b7e88caeebcc217</v>
       </c>
       <c r="B2" t="str">
         <v>Amrendra Bahubali</v>
@@ -442,62 +442,39 @@
         <v>king</v>
       </c>
       <c r="F2" t="str">
-        <v>64d275472876b66b40a62e22 ; 64d275752876b66b40a62e28</v>
+        <v>64d275752876b66b40a62e28 ; 64d275472876b66b40a62e22</v>
       </c>
       <c r="G2" t="str">
-        <v>http://localhost:3000/img/amrendra.jpg ; http://localhost:3000/img/amrendra-2.webp</v>
+        <v>http://localhost:3000/img/amrendra-2.webp ; http://localhost:3000/img/amrendra.jpg</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>64d271f52928446e16714194</v>
+        <v>64d67a92d56affd78effbea4</v>
       </c>
       <c r="B3" t="str">
-        <v>Mahendra Bahubali</v>
+        <v>Katappa</v>
       </c>
       <c r="C3">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D3" t="str">
         <v>male</v>
       </c>
       <c r="E3" t="str">
-        <v>prince</v>
+        <v>knight</v>
       </c>
       <c r="F3" t="str">
-        <v>64d272c461e8fe1d4b469512 ; 64d2761c2876b66b40a62e37</v>
+        <v>64d275752876b66b40a62e28 ; 64d275ac2876b66b40a62e2e</v>
       </c>
       <c r="G3" t="str">
-        <v>http://localhost:3000/img/mahendra.jpg</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>64d2750e2876b66b40a62e1a</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Katappa</v>
-      </c>
-      <c r="C4">
-        <v>70</v>
-      </c>
-      <c r="D4" t="str">
-        <v>male</v>
-      </c>
-      <c r="E4" t="str">
-        <v>knight</v>
-      </c>
-      <c r="F4" t="str">
-        <v>64d275042876b66b40a62e17 ; 64d275ac2876b66b40a62e2e</v>
-      </c>
-      <c r="G4" t="str">
         <v>http://localhost:3000/img/katappa.jpg</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>